<commit_message>
Componentes ADCS: Precio Masa, Potencia
</commit_message>
<xml_diff>
--- a/ADCS/Component info.xlsx
+++ b/ADCS/Component info.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\diego\Documents\MEng Space Systems (Local)\2. CE1\Educational-CubeSat-Design\ADCS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B5E6D6D-E12D-4E25-8A2D-D8E43DDBD101}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{000FDA11-0B41-47B5-A2E8-5BF63431CF34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-105" windowWidth="29040" windowHeight="15840" xr2:uid="{E0DC4ABA-2EDA-4F01-86D2-414EB06C3538}"/>
   </bookViews>
@@ -1035,7 +1035,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1064,12 +1064,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1151,7 +1145,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1265,6 +1259,18 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1289,32 +1295,23 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2342,7 +2339,7 @@
   <dimension ref="A1:Y37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q2" sqref="Q2:Q3"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2369,10 +2366,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="54" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="50"/>
+      <c r="B1" s="54"/>
       <c r="C1" s="9" t="s">
         <v>48</v>
       </c>
@@ -2435,10 +2432,10 @@
       </c>
     </row>
     <row r="2" spans="1:25" ht="15.6" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="48" t="s">
+      <c r="A2" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="59" t="s">
+      <c r="B2" s="55" t="s">
         <v>77</v>
       </c>
       <c r="C2" s="38">
@@ -2450,7 +2447,7 @@
       <c r="E2" s="38" t="s">
         <v>86</v>
       </c>
-      <c r="F2" s="55" t="s">
+      <c r="F2" s="43" t="s">
         <v>83</v>
       </c>
       <c r="G2" s="38">
@@ -2483,10 +2480,10 @@
       <c r="P2" s="22" t="s">
         <v>82</v>
       </c>
-      <c r="Q2" s="43" t="s">
+      <c r="Q2" s="47" t="s">
         <v>81</v>
       </c>
-      <c r="R2" s="55" t="s">
+      <c r="R2" s="43" t="s">
         <v>7</v>
       </c>
       <c r="S2" s="38" t="s">
@@ -2502,8 +2499,8 @@
       </c>
     </row>
     <row r="3" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="48"/>
-      <c r="B3" s="52"/>
+      <c r="A3" s="52"/>
+      <c r="B3" s="56"/>
       <c r="C3" s="40">
         <v>1</v>
       </c>
@@ -2540,14 +2537,14 @@
       <c r="N3" s="40">
         <v>0.5</v>
       </c>
-      <c r="O3" s="56" t="s">
+      <c r="O3" s="44" t="s">
         <v>85</v>
       </c>
-      <c r="P3" s="57" t="str">
+      <c r="P3" s="45" t="str">
         <f>P6</f>
         <v>-30 - +85</v>
       </c>
-      <c r="Q3" s="46"/>
+      <c r="Q3" s="50"/>
       <c r="R3" s="40"/>
       <c r="S3" s="40"/>
       <c r="T3" s="40"/>
@@ -2555,7 +2552,7 @@
       <c r="Y3" s="19"/>
     </row>
     <row r="4" spans="1:25" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="53"/>
+      <c r="A4" s="57"/>
       <c r="B4" s="27" t="s">
         <v>20</v>
       </c>
@@ -2621,10 +2618,10 @@
       </c>
     </row>
     <row r="5" spans="1:25" ht="29.4" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="48" t="s">
+      <c r="A5" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="47" t="s">
+      <c r="B5" s="51" t="s">
         <v>25</v>
       </c>
       <c r="C5" s="8">
@@ -2642,7 +2639,7 @@
       <c r="G5" s="8">
         <v>6</v>
       </c>
-      <c r="H5" s="43" t="s">
+      <c r="H5" s="47" t="s">
         <v>46</v>
       </c>
       <c r="I5" s="8" t="s">
@@ -2669,7 +2666,7 @@
       <c r="P5" s="22" t="s">
         <v>74</v>
       </c>
-      <c r="Q5" s="43" t="s">
+      <c r="Q5" s="47" t="s">
         <v>70</v>
       </c>
       <c r="R5" s="8"/>
@@ -2684,8 +2681,8 @@
       </c>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A6" s="48"/>
-      <c r="B6" s="48"/>
+      <c r="A6" s="52"/>
+      <c r="B6" s="52"/>
       <c r="C6" s="4">
         <v>3</v>
       </c>
@@ -2702,7 +2699,7 @@
         <f>1.85*0.001*(13.4*13.4*4.5)*1.5</f>
         <v>2.2422554999999997</v>
       </c>
-      <c r="H6" s="44"/>
+      <c r="H6" s="48"/>
       <c r="I6" s="4" t="s">
         <v>56</v>
       </c>
@@ -2727,7 +2724,7 @@
       <c r="P6" s="34" t="s">
         <v>101</v>
       </c>
-      <c r="Q6" s="44"/>
+      <c r="Q6" s="48"/>
       <c r="R6" s="4"/>
       <c r="S6" s="4"/>
       <c r="T6" s="4"/>
@@ -2740,8 +2737,8 @@
       </c>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A7" s="48"/>
-      <c r="B7" s="49"/>
+      <c r="A7" s="52"/>
+      <c r="B7" s="53"/>
       <c r="C7" s="4">
         <v>3</v>
       </c>
@@ -2757,7 +2754,7 @@
       <c r="G7" s="4">
         <v>10</v>
       </c>
-      <c r="H7" s="46"/>
+      <c r="H7" s="50"/>
       <c r="I7" s="4" t="s">
         <v>55</v>
       </c>
@@ -2782,7 +2779,7 @@
       <c r="P7" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="Q7" s="44"/>
+      <c r="Q7" s="48"/>
       <c r="R7" s="4"/>
       <c r="S7" s="4"/>
       <c r="T7" s="4"/>
@@ -2795,7 +2792,7 @@
       </c>
     </row>
     <row r="8" spans="1:25" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="49"/>
+      <c r="A8" s="53"/>
       <c r="B8" s="3" t="s">
         <v>29</v>
       </c>
@@ -2833,7 +2830,7 @@
         <v>95</v>
       </c>
       <c r="N8" s="14">
-        <v>80</v>
+        <v>120</v>
       </c>
       <c r="O8" s="16" t="s">
         <v>58</v>
@@ -2863,11 +2860,11 @@
       </c>
     </row>
     <row r="10" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F10" s="45" t="s">
+      <c r="F10" s="49" t="s">
         <v>61</v>
       </c>
-      <c r="G10" s="45"/>
-      <c r="H10" s="45"/>
+      <c r="G10" s="49"/>
+      <c r="H10" s="49"/>
       <c r="I10" s="30"/>
       <c r="L10" s="28" t="s">
         <v>65</v>
@@ -2887,7 +2884,7 @@
       <c r="F11" s="17" t="s">
         <v>88</v>
       </c>
-      <c r="G11" s="30">
+      <c r="G11" s="60">
         <f>C2*G2+C5*G5+C6*G6+C7*G7+C8*G8+C3*G3+G4*C4</f>
         <v>68.226766499999997</v>
       </c>
@@ -2901,7 +2898,7 @@
       <c r="M11" s="30"/>
       <c r="N11" s="30">
         <f>C2*N2+N5*C5+N6*C6+N7*C7+N8*C8+N3*C3+N4*C4</f>
-        <v>612.36</v>
+        <v>692.36</v>
       </c>
       <c r="O11" s="31" t="s">
         <v>64</v>
@@ -2929,7 +2926,7 @@
       <c r="M12" s="30"/>
       <c r="N12" s="30">
         <f>N10-N11</f>
-        <v>-162.36000000000001</v>
+        <v>-242.36</v>
       </c>
       <c r="O12" s="31" t="s">
         <v>64</v>
@@ -2942,7 +2939,7 @@
       <c r="F13" s="36" t="s">
         <v>90</v>
       </c>
-      <c r="G13" s="58" t="s">
+      <c r="G13" s="46" t="s">
         <v>104</v>
       </c>
       <c r="H13" s="10" t="s">
@@ -3045,10 +3042,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="54" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="50"/>
+      <c r="B1" s="54"/>
       <c r="C1" s="9" t="s">
         <v>48</v>
       </c>
@@ -3111,10 +3108,10 @@
       </c>
     </row>
     <row r="2" spans="1:25" ht="15.6" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="48" t="s">
+      <c r="A2" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="51" t="s">
+      <c r="B2" s="58" t="s">
         <v>77</v>
       </c>
       <c r="C2" s="38">
@@ -3126,7 +3123,7 @@
       <c r="E2" s="38" t="s">
         <v>86</v>
       </c>
-      <c r="F2" s="55" t="s">
+      <c r="F2" s="43" t="s">
         <v>83</v>
       </c>
       <c r="G2" s="38">
@@ -3162,7 +3159,7 @@
       <c r="Q2" s="38" t="s">
         <v>81</v>
       </c>
-      <c r="R2" s="55" t="s">
+      <c r="R2" s="43" t="s">
         <v>7</v>
       </c>
       <c r="S2" s="38" t="s">
@@ -3178,8 +3175,8 @@
       </c>
     </row>
     <row r="3" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="48"/>
-      <c r="B3" s="52"/>
+      <c r="A3" s="52"/>
+      <c r="B3" s="56"/>
       <c r="C3" s="40">
         <v>1</v>
       </c>
@@ -3216,10 +3213,10 @@
       <c r="N3" s="40">
         <v>0.5</v>
       </c>
-      <c r="O3" s="56" t="s">
+      <c r="O3" s="44" t="s">
         <v>85</v>
       </c>
-      <c r="P3" s="57" t="str">
+      <c r="P3" s="45" t="str">
         <f>P7</f>
         <v>-30 - +85</v>
       </c>
@@ -3231,7 +3228,7 @@
       <c r="Y3" s="19"/>
     </row>
     <row r="4" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="48"/>
+      <c r="A4" s="52"/>
       <c r="B4" s="27" t="s">
         <v>20</v>
       </c>
@@ -3292,7 +3289,7 @@
       <c r="Y4" s="19"/>
     </row>
     <row r="5" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="53"/>
+      <c r="A5" s="57"/>
       <c r="B5" s="42" t="s">
         <v>23</v>
       </c>
@@ -3352,10 +3349,10 @@
       </c>
     </row>
     <row r="6" spans="1:25" ht="29.4" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="48" t="s">
+      <c r="A6" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="47" t="s">
+      <c r="B6" s="51" t="s">
         <v>25</v>
       </c>
       <c r="C6" s="38">
@@ -3373,7 +3370,7 @@
       <c r="G6" s="38">
         <v>6</v>
       </c>
-      <c r="H6" s="43" t="s">
+      <c r="H6" s="47" t="s">
         <v>46</v>
       </c>
       <c r="I6" s="38" t="s">
@@ -3400,7 +3397,7 @@
       <c r="P6" s="22" t="s">
         <v>74</v>
       </c>
-      <c r="Q6" s="43" t="s">
+      <c r="Q6" s="47" t="s">
         <v>70</v>
       </c>
       <c r="R6" s="38"/>
@@ -3415,8 +3412,8 @@
       </c>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A7" s="48"/>
-      <c r="B7" s="48"/>
+      <c r="A7" s="52"/>
+      <c r="B7" s="52"/>
       <c r="C7" s="39">
         <v>3</v>
       </c>
@@ -3433,7 +3430,7 @@
         <f>1.85*0.001*(13.4*13.4*4.5)*1.5</f>
         <v>2.2422554999999997</v>
       </c>
-      <c r="H7" s="44"/>
+      <c r="H7" s="48"/>
       <c r="I7" s="39" t="s">
         <v>56</v>
       </c>
@@ -3458,7 +3455,7 @@
       <c r="P7" s="34" t="s">
         <v>101</v>
       </c>
-      <c r="Q7" s="44"/>
+      <c r="Q7" s="48"/>
       <c r="R7" s="39"/>
       <c r="S7" s="39"/>
       <c r="T7" s="39"/>
@@ -3471,8 +3468,8 @@
       </c>
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A8" s="48"/>
-      <c r="B8" s="49"/>
+      <c r="A8" s="52"/>
+      <c r="B8" s="53"/>
       <c r="C8" s="39">
         <v>3</v>
       </c>
@@ -3488,7 +3485,7 @@
       <c r="G8" s="39">
         <v>10</v>
       </c>
-      <c r="H8" s="46"/>
+      <c r="H8" s="50"/>
       <c r="I8" s="39" t="s">
         <v>55</v>
       </c>
@@ -3513,7 +3510,7 @@
       <c r="P8" s="39" t="s">
         <v>46</v>
       </c>
-      <c r="Q8" s="44"/>
+      <c r="Q8" s="48"/>
       <c r="R8" s="39"/>
       <c r="S8" s="39"/>
       <c r="T8" s="39"/>
@@ -3526,7 +3523,7 @@
       </c>
     </row>
     <row r="9" spans="1:25" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A9" s="49"/>
+      <c r="A9" s="53"/>
       <c r="B9" s="41" t="s">
         <v>29</v>
       </c>
@@ -3594,11 +3591,11 @@
       </c>
     </row>
     <row r="11" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F11" s="45" t="s">
+      <c r="F11" s="49" t="s">
         <v>61</v>
       </c>
-      <c r="G11" s="45"/>
-      <c r="H11" s="45"/>
+      <c r="G11" s="49"/>
+      <c r="H11" s="49"/>
       <c r="I11" s="30"/>
       <c r="L11" s="28" t="s">
         <v>65</v>
@@ -3673,7 +3670,7 @@
       <c r="F14" s="36" t="s">
         <v>90</v>
       </c>
-      <c r="G14" s="58" t="s">
+      <c r="G14" s="46" t="s">
         <v>104</v>
       </c>
       <c r="H14" s="10" t="s">
@@ -3749,10 +3746,10 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:23" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="54" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="50"/>
+      <c r="B1" s="54"/>
       <c r="C1" s="9" t="s">
         <v>48</v>
       </c>
@@ -3809,10 +3806,10 @@
       </c>
     </row>
     <row r="2" spans="1:23" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="48" t="s">
+      <c r="A2" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="48" t="s">
+      <c r="B2" s="52" t="s">
         <v>20</v>
       </c>
       <c r="C2" s="4">
@@ -3852,8 +3849,8 @@
       </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A3" s="48"/>
-      <c r="B3" s="49"/>
+      <c r="A3" s="52"/>
+      <c r="B3" s="53"/>
       <c r="C3" s="5">
         <v>1</v>
       </c>
@@ -3888,7 +3885,7 @@
       </c>
     </row>
     <row r="4" spans="1:23" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="48"/>
+      <c r="A4" s="52"/>
       <c r="B4" s="27" t="s">
         <v>77</v>
       </c>
@@ -3927,7 +3924,7 @@
       <c r="S4" s="2"/>
     </row>
     <row r="5" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="53"/>
+      <c r="A5" s="57"/>
       <c r="B5" s="7" t="s">
         <v>23</v>
       </c>
@@ -3981,10 +3978,10 @@
       </c>
     </row>
     <row r="6" spans="1:23" ht="43.8" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="48" t="s">
+      <c r="A6" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="47" t="s">
+      <c r="B6" s="51" t="s">
         <v>25</v>
       </c>
       <c r="C6" s="8">
@@ -4023,7 +4020,7 @@
       <c r="N6" s="22" t="s">
         <v>74</v>
       </c>
-      <c r="O6" s="43" t="s">
+      <c r="O6" s="47" t="s">
         <v>70</v>
       </c>
       <c r="P6" s="8"/>
@@ -4035,8 +4032,8 @@
       </c>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A7" s="48"/>
-      <c r="B7" s="48"/>
+      <c r="A7" s="52"/>
+      <c r="B7" s="52"/>
       <c r="C7" s="4">
         <v>3</v>
       </c>
@@ -4070,7 +4067,7 @@
       <c r="N7" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="O7" s="44"/>
+      <c r="O7" s="48"/>
       <c r="P7" s="4"/>
       <c r="Q7" s="4"/>
       <c r="R7" s="4"/>
@@ -4080,8 +4077,8 @@
       </c>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A8" s="48"/>
-      <c r="B8" s="48"/>
+      <c r="A8" s="52"/>
+      <c r="B8" s="52"/>
       <c r="C8" s="4">
         <v>3</v>
       </c>
@@ -4118,15 +4115,15 @@
       <c r="N8" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="O8" s="44"/>
+      <c r="O8" s="48"/>
       <c r="P8" s="4"/>
       <c r="Q8" s="4"/>
       <c r="R8" s="4"/>
       <c r="S8" s="2"/>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A9" s="48"/>
-      <c r="B9" s="49"/>
+      <c r="A9" s="52"/>
+      <c r="B9" s="53"/>
       <c r="C9" s="5"/>
       <c r="D9" s="5" t="s">
         <v>35</v>
@@ -4157,8 +4154,8 @@
       </c>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A10" s="48"/>
-      <c r="B10" s="54" t="s">
+      <c r="A10" s="52"/>
+      <c r="B10" s="59" t="s">
         <v>29</v>
       </c>
       <c r="C10" s="6" t="s">
@@ -4195,8 +4192,8 @@
       </c>
     </row>
     <row r="11" spans="1:23" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A11" s="49"/>
-      <c r="B11" s="49"/>
+      <c r="A11" s="53"/>
+      <c r="B11" s="53"/>
       <c r="C11" s="14">
         <v>2</v>
       </c>

</xml_diff>